<commit_message>
add hours spent for sprint 9 of the first week
</commit_message>
<xml_diff>
--- a/feebacks-timesheets/Sprint9_Timesheet.xlsx
+++ b/feebacks-timesheets/Sprint9_Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asarpa\Desktop\thesis\feebacks-timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A9A858-C150-4194-A330-9AE79BD27F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A633B81-3F49-4915-8A4A-1FC1B6B32D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -336,6 +336,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -360,7 +361,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +591,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -608,39 +608,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:11" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="12"/>
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6" s="13">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="12"/>
@@ -781,7 +781,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G8" s="13">
         <v>0</v>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="13">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="13"/>
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="13">
         <v>0</v>
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="13">
         <v>0</v>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I9" s="13">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D10" s="12">
         <v>0</v>
@@ -863,11 +863,11 @@
       </c>
       <c r="B11" s="13">
         <f>SUM(B5:B10)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C11" s="13">
         <f t="shared" ref="C11:I11" si="0">SUM(C5:C10)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D11" s="13">
         <f>SUM(D5:D10)</f>
@@ -875,11 +875,11 @@
       </c>
       <c r="E11" s="13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
@@ -887,100 +887,100 @@
       </c>
       <c r="H11" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -992,176 +992,176 @@
       <c r="C21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="16">
         <v>8</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
     </row>
     <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="16">
         <v>2</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="16">
         <v>2</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
     </row>
     <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="28">
+      <c r="B25" s="16">
         <v>2</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="28"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="16">
         <v>2</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="28"/>
     </row>
     <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="28">
+      <c r="B27" s="16">
         <v>3</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="28"/>
     </row>
     <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="16">
         <v>2</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="28"/>
     </row>
     <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="16">
         <v>5</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="28"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="2"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
       <c r="B32" s="2"/>
       <c r="C32" s="14"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="2"/>
       <c r="C33" s="14"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:9" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add data and retrospective of sprint 9
</commit_message>
<xml_diff>
--- a/feebacks-timesheets/Sprint9_Timesheet.xlsx
+++ b/feebacks-timesheets/Sprint9_Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asarpa\Desktop\thesis\feebacks-timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A633B81-3F49-4915-8A4A-1FC1B6B32D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6679E5AF-81BA-47AC-B97B-7BAF5CE53EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Amedeo</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>see consultants' statistic widget</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>required a lot of effort unexpected, in particular for the grpc connection</t>
+  </si>
+  <si>
+    <t>yes, underestimated, new_func</t>
   </si>
 </sst>
 </file>
@@ -590,8 +599,8 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -600,7 +609,7 @@
     <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="32.42578125" bestFit="1" customWidth="1"/>
@@ -682,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E5" s="13">
         <v>0</v>
@@ -722,10 +731,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I6" s="13">
         <v>0</v>
@@ -759,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="13">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="12"/>
@@ -778,10 +787,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="13">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F8" s="13">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G8" s="13">
         <v>0</v>
@@ -806,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="13">
         <v>1</v>
@@ -815,10 +824,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H9" s="13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I9" s="13">
         <v>0</v>
@@ -834,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="12">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D10" s="12">
         <v>0</v>
@@ -867,31 +876,31 @@
       </c>
       <c r="C11" s="13">
         <f t="shared" ref="C11:I11" si="0">SUM(C5:C10)</f>
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D11" s="13">
         <f>SUM(D5:D10)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E11" s="13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F11" s="13">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H11" s="13">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -1006,8 +1015,12 @@
       <c r="B22" s="16">
         <v>8</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="24"/>
+      <c r="C22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>37</v>
+      </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
@@ -1019,9 +1032,11 @@
         <v>23</v>
       </c>
       <c r="B23" s="16">
-        <v>2</v>
-      </c>
-      <c r="C23" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
       <c r="F23" s="25"/>
@@ -1036,7 +1051,9 @@
       <c r="B24" s="16">
         <v>2</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
@@ -1051,7 +1068,9 @@
       <c r="B25" s="16">
         <v>2</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
@@ -1066,7 +1085,9 @@
       <c r="B26" s="16">
         <v>2</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
@@ -1081,7 +1102,9 @@
       <c r="B27" s="16">
         <v>3</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
@@ -1096,7 +1119,9 @@
       <c r="B28" s="16">
         <v>2</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
@@ -1111,7 +1136,9 @@
       <c r="B29" s="16">
         <v>5</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>

</xml_diff>